<commit_message>
assembled some janky version of mrp backend
</commit_message>
<xml_diff>
--- a/data-parsing/All Shibaura PO/Allpos/po_numbers.xlsx
+++ b/data-parsing/All Shibaura PO/Allpos/po_numbers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMC\SynologyDrive\Administrative\PO Processing\All Shibaura PO\Allpos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMC\Documents\My Repos\MRP-Planning\data-parsing\All Shibaura PO\Allpos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFC67D3A-AE42-48E6-B74D-EBCB0220291C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2C857B-C98A-4EF5-9FB7-66DCD88212FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2C47A718-98E0-4021-8834-4D5B504F3E57}"/>
   </bookViews>
@@ -12231,13 +12231,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98240824-809F-40E7-A589-57DFA5FA97AF}">
   <dimension ref="A1:B1897"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1845" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1858" sqref="F1858"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>